<commit_message>
the form for adding a supplier is change to have a better look the main map now has a locate plugin to find the user location the base template now has a link to the main map the data for the suppliers is updated and now includes the lat and lon
</commit_message>
<xml_diff>
--- a/proveeagro/data/suppliers_medellin.xlsx
+++ b/proveeagro/data/suppliers_medellin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Documents\vs-code\ppi_proveeagro\proveeagro\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\VS_Code\ppi_proveeagro\proveeagro\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358DE5AE-EEC2-43D7-B70E-BD8EFE377BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8971BB73-34D3-4AA1-8C90-3C709D5D818F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D8556FE-D2CF-4229-94F1-9AD660868E54}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6D8556FE-D2CF-4229-94F1-9AD660868E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="419">
   <si>
     <t>department</t>
   </si>
@@ -1041,6 +1041,345 @@
   </si>
   <si>
     <t>address2</t>
+  </si>
+  <si>
+    <t>6.2395758,-75.570565</t>
+  </si>
+  <si>
+    <t>6.2900161,-75.5717382</t>
+  </si>
+  <si>
+    <t>6.2722815,-75.5737099</t>
+  </si>
+  <si>
+    <t>6.297725499999999,-75.5664015</t>
+  </si>
+  <si>
+    <t>6.2382773,-75.5707746</t>
+  </si>
+  <si>
+    <t>6.2300007,-75.5816188</t>
+  </si>
+  <si>
+    <t>6.2934904,-75.54169069999999</t>
+  </si>
+  <si>
+    <t>6.2457302,-75.5607383</t>
+  </si>
+  <si>
+    <t>6.250465999999999,-75.5683201</t>
+  </si>
+  <si>
+    <t>6.209798999999999,-75.56590539999999</t>
+  </si>
+  <si>
+    <t>6.279211699999999,-75.63454949999999</t>
+  </si>
+  <si>
+    <t>6.277932799999999,-75.63581789999999</t>
+  </si>
+  <si>
+    <t>6.257022399999999,-75.5697711</t>
+  </si>
+  <si>
+    <t>6.2392587,-75.57008689999999</t>
+  </si>
+  <si>
+    <t>6.2503094,-75.5704198</t>
+  </si>
+  <si>
+    <t>6.2787933,-75.5029909</t>
+  </si>
+  <si>
+    <t>6.2469039,-75.5730894</t>
+  </si>
+  <si>
+    <t>6.306056,-75.5599052</t>
+  </si>
+  <si>
+    <t>6.225079999999999,-75.5714893</t>
+  </si>
+  <si>
+    <t>6.2939302,-75.5588908</t>
+  </si>
+  <si>
+    <t>6.246724599999999,-75.5986891</t>
+  </si>
+  <si>
+    <t>6.2357604,-75.5613024</t>
+  </si>
+  <si>
+    <t>6.206191,-75.56433799999999</t>
+  </si>
+  <si>
+    <t>6.2559607,-75.5742808</t>
+  </si>
+  <si>
+    <t>6.2559193,-75.5742191</t>
+  </si>
+  <si>
+    <t>6.201767,-75.581246</t>
+  </si>
+  <si>
+    <t>6.246788599999999,-75.5600087</t>
+  </si>
+  <si>
+    <t>6.2462294,-75.55874639999999</t>
+  </si>
+  <si>
+    <t>6.2859551,-75.5624029</t>
+  </si>
+  <si>
+    <t>6.263834200000001,-75.600292</t>
+  </si>
+  <si>
+    <t>6.164727,-75.6171911</t>
+  </si>
+  <si>
+    <t>6.2522294,-75.59162169999999</t>
+  </si>
+  <si>
+    <t>6.247189,-75.5593847</t>
+  </si>
+  <si>
+    <t>6.2706578,-75.5767491</t>
+  </si>
+  <si>
+    <t>6.248574,-75.58389199999999</t>
+  </si>
+  <si>
+    <t>6.2121904,-75.59469229999999</t>
+  </si>
+  <si>
+    <t>6.256249299999999,-75.5806589</t>
+  </si>
+  <si>
+    <t>6.224914399999999,-75.57493509999999</t>
+  </si>
+  <si>
+    <t>6.198575399999999,-75.5567906</t>
+  </si>
+  <si>
+    <t>6.218830800000001,-75.5833193</t>
+  </si>
+  <si>
+    <t>6.2612102,-75.5897096</t>
+  </si>
+  <si>
+    <t>6.1974567,-75.558218</t>
+  </si>
+  <si>
+    <t>6.1974022,-75.55810210000001</t>
+  </si>
+  <si>
+    <t>6.228770099999999,-75.57781969999999</t>
+  </si>
+  <si>
+    <t>6.2486956,-75.5664741</t>
+  </si>
+  <si>
+    <t>6.2383719,-75.5472138</t>
+  </si>
+  <si>
+    <t>6.2327678,-75.6041795</t>
+  </si>
+  <si>
+    <t>6.268424,-75.604331</t>
+  </si>
+  <si>
+    <t>6.2648055,-75.55545649999999</t>
+  </si>
+  <si>
+    <t>6.252327999999999,-75.5671574</t>
+  </si>
+  <si>
+    <t>6.1987146,-75.5746333</t>
+  </si>
+  <si>
+    <t>6.238475999999999,-75.5718591</t>
+  </si>
+  <si>
+    <t>6.229799,-75.5701449</t>
+  </si>
+  <si>
+    <t>6.2732086,-75.5935341</t>
+  </si>
+  <si>
+    <t>6.2838629,-75.5842182</t>
+  </si>
+  <si>
+    <t>6.1546916,-75.6284391</t>
+  </si>
+  <si>
+    <t>6.196852,-75.574351</t>
+  </si>
+  <si>
+    <t>6.239482799999999,-75.5877758</t>
+  </si>
+  <si>
+    <t>6.202830199999999,-75.5813411</t>
+  </si>
+  <si>
+    <t>6.2597532,-75.5714203</t>
+  </si>
+  <si>
+    <t>6.245793399999999,-75.569035</t>
+  </si>
+  <si>
+    <t>6.255808000000001,-75.57943259999999</t>
+  </si>
+  <si>
+    <t>6.2292663,-75.5630018</t>
+  </si>
+  <si>
+    <t>6.3014278,-75.56389949999999</t>
+  </si>
+  <si>
+    <t>6.2450608,-75.55917</t>
+  </si>
+  <si>
+    <t>6.255082400000001,-75.57389420000001</t>
+  </si>
+  <si>
+    <t>6.2129594,-75.5591245</t>
+  </si>
+  <si>
+    <t>6.196598799999999,-75.5741608</t>
+  </si>
+  <si>
+    <t>6.2210934,-75.57514920000001</t>
+  </si>
+  <si>
+    <t>6.2333751,-75.6049993</t>
+  </si>
+  <si>
+    <t>6.249149399999999,-75.5843197</t>
+  </si>
+  <si>
+    <t>6.3107843,-75.5517162</t>
+  </si>
+  <si>
+    <t>6.214498400000001,-75.5702901</t>
+  </si>
+  <si>
+    <t>6.240684,-75.5528321</t>
+  </si>
+  <si>
+    <t>6.257733,-75.5850359</t>
+  </si>
+  <si>
+    <t>6.2474361,-75.5679083</t>
+  </si>
+  <si>
+    <t>6.263317499999999,-75.5888405</t>
+  </si>
+  <si>
+    <t>6.245179599999999,-75.6004188</t>
+  </si>
+  <si>
+    <t>6.181784899999999,-75.56942599999999</t>
+  </si>
+  <si>
+    <t>6.2049639,-75.601315</t>
+  </si>
+  <si>
+    <t>6.2225611,-75.49548639999999</t>
+  </si>
+  <si>
+    <t>6.2491793,-75.5724287</t>
+  </si>
+  <si>
+    <t>6.241613900000001,-75.5828077</t>
+  </si>
+  <si>
+    <t>6.1862521,-75.6561581</t>
+  </si>
+  <si>
+    <t>6.1815767,-75.5721092</t>
+  </si>
+  <si>
+    <t>6.286264,-75.6448162</t>
+  </si>
+  <si>
+    <t>6.302100200000001,-75.5564478</t>
+  </si>
+  <si>
+    <t>6.2096922,-75.5763671</t>
+  </si>
+  <si>
+    <t>6.2459225,-75.59665369999999</t>
+  </si>
+  <si>
+    <t>6.1899675,-75.6009213</t>
+  </si>
+  <si>
+    <t>6.209024899999999,-75.5855082</t>
+  </si>
+  <si>
+    <t>6.2582486,-75.60377749999999</t>
+  </si>
+  <si>
+    <t>6.254547899999999,-75.5744706</t>
+  </si>
+  <si>
+    <t>6.2848251,-75.5583968</t>
+  </si>
+  <si>
+    <t>6.173081499999999,-75.562692</t>
+  </si>
+  <si>
+    <t>6.2488123,-75.6085465</t>
+  </si>
+  <si>
+    <t>6.2973716,-75.5656625</t>
+  </si>
+  <si>
+    <t>6.2305742,-75.6062587</t>
+  </si>
+  <si>
+    <t>6.2422679,-75.5553394</t>
+  </si>
+  <si>
+    <t>6.273851899999999,-75.55803</t>
+  </si>
+  <si>
+    <t>6.213566900000001,-75.5841315</t>
+  </si>
+  <si>
+    <t>6.2911461,-75.57184769999999</t>
+  </si>
+  <si>
+    <t>6.250245,-75.5908299</t>
+  </si>
+  <si>
+    <t>6.2183451,-75.57961300000001</t>
+  </si>
+  <si>
+    <t>6.238572899999999,-75.59568800000001</t>
+  </si>
+  <si>
+    <t>6.2748288,-75.5834102</t>
+  </si>
+  <si>
+    <t>6.275536900000001,-75.5967924</t>
+  </si>
+  <si>
+    <t>6.280470500000001,-75.5888536</t>
+  </si>
+  <si>
+    <t>6.2549334,-75.6203996</t>
+  </si>
+  <si>
+    <t>6.290986999999999,-75.5535755</t>
+  </si>
+  <si>
+    <t>6.2331902,-75.5739454</t>
+  </si>
+  <si>
+    <t>6.208302799999999,-75.5714953</t>
+  </si>
+  <si>
+    <t>coordinates</t>
   </si>
 </sst>
 </file>
@@ -1100,16 +1439,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A487A160-4BF0-4276-976C-ECCA1635D26E}" name="Tabla1" displayName="Tabla1" ref="A1:G119" totalsRowShown="0">
-  <autoFilter ref="A1:G119" xr:uid="{A487A160-4BF0-4276-976C-ECCA1635D26E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A487A160-4BF0-4276-976C-ECCA1635D26E}" name="Tabla1" displayName="Tabla1" ref="A1:H119" totalsRowShown="0">
+  <autoFilter ref="A1:H119" xr:uid="{A487A160-4BF0-4276-976C-ECCA1635D26E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H119">
     <sortCondition ref="A1:A119"/>
   </sortState>
-  <tableColumns count="7">
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{8D266C73-2FA1-4EF8-A5BC-B85B8973220E}" name="name"/>
     <tableColumn id="7" xr3:uid="{C2A46D66-2197-4E03-BD99-1DCFFDC71FC6}" name="address" dataDxfId="0">
       <calculatedColumnFormula>TRIM(Tabla1[[#This Row],[address2]])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="10" xr3:uid="{A6FC2ECB-9CDE-4E28-A598-CF3E733A3B7E}" name="coordinates"/>
     <tableColumn id="2" xr3:uid="{E3982764-83B8-4522-8585-0F95BE5CFBF6}" name="address2"/>
     <tableColumn id="3" xr3:uid="{F9C1C376-9912-4214-9BA3-3F8640625EE3}" name="email"/>
     <tableColumn id="4" xr3:uid="{697EA875-A3F7-4570-85C2-9B6B4BE9AE74}" name="phone"/>
@@ -1121,9 +1461,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1161,7 +1501,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1267,7 +1607,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1409,7 +1749,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1417,23 +1757,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46769F8C-7CE4-442C-A862-3CDF4EA09A62}">
-  <dimension ref="A1:G119"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.5703125" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>304</v>
       </c>
@@ -1441,22 +1782,25 @@
         <v>303</v>
       </c>
       <c r="C1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D1" t="s">
         <v>305</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>302</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>301</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>187</v>
       </c>
@@ -1465,22 +1809,25 @@
         <v>Carrera 46 # 39 9</v>
       </c>
       <c r="C2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2" t="s">
         <v>70</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>274</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2321891</v>
       </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
       <c r="G2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>201</v>
       </c>
@@ -1489,22 +1836,25 @@
         <v>Carrera 67 # 95 33</v>
       </c>
       <c r="C3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>288</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>3205566918</v>
       </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
       <c r="G3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -1513,22 +1863,25 @@
         <v>Carrera 64 C # 72 - 157</v>
       </c>
       <c r="C4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>245</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>4455555</v>
       </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
       <c r="G4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -1538,22 +1891,25 @@
 Interior164</v>
       </c>
       <c r="C5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>245</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>4455555</v>
       </c>
-      <c r="F5" t="s">
-        <v>3</v>
-      </c>
       <c r="G5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>132</v>
       </c>
@@ -1562,22 +1918,25 @@
         <v>Carrera 46 # 37 - 63</v>
       </c>
       <c r="C6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>245</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>4455555</v>
       </c>
-      <c r="F6" t="s">
-        <v>3</v>
-      </c>
       <c r="G6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>198</v>
       </c>
@@ -1586,22 +1945,25 @@
         <v>Carrera 58 A # 29 84</v>
       </c>
       <c r="C7" t="s">
+        <v>311</v>
+      </c>
+      <c r="D7" t="s">
         <v>81</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>285</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>3148321396</v>
       </c>
-      <c r="F7" t="s">
-        <v>3</v>
-      </c>
       <c r="G7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>189</v>
       </c>
@@ -1610,22 +1972,25 @@
         <v>Carrera 31 A # 102 B 207</v>
       </c>
       <c r="C8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D8" t="s">
         <v>72</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>276</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>4637049</v>
       </c>
-      <c r="F8" t="s">
-        <v>3</v>
-      </c>
       <c r="G8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>200</v>
       </c>
@@ -1634,22 +1999,25 @@
         <v>Carrera 40 # 49 91</v>
       </c>
       <c r="C9" t="s">
+        <v>313</v>
+      </c>
+      <c r="D9" t="s">
         <v>83</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>287</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>3195371939</v>
       </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
       <c r="G9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>179</v>
       </c>
@@ -1659,22 +2027,25 @@
 INTERIOR146</v>
       </c>
       <c r="C10" t="s">
+        <v>309</v>
+      </c>
+      <c r="D10" t="s">
         <v>62</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>268</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>6378080</v>
       </c>
-      <c r="F10" t="s">
-        <v>3</v>
-      </c>
       <c r="G10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>122</v>
       </c>
@@ -1683,22 +2054,25 @@
         <v>Carrera 51 # 6 Sur 95</v>
       </c>
       <c r="C11" t="s">
+        <v>314</v>
+      </c>
+      <c r="D11" t="s">
         <v>5</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>240</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>4481349</v>
       </c>
-      <c r="F11" t="s">
-        <v>3</v>
-      </c>
       <c r="G11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -1707,22 +2081,25 @@
         <v>Calle 10 a # 36 a este- 163</v>
       </c>
       <c r="C12" t="s">
+        <v>315</v>
+      </c>
+      <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>247</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>3147599973</v>
       </c>
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
       <c r="G12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>203</v>
       </c>
@@ -1731,22 +2108,25 @@
         <v>Calle 63 # 129 A 8</v>
       </c>
       <c r="C13" t="s">
+        <v>316</v>
+      </c>
+      <c r="D13" t="s">
         <v>86</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>290</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>6044278821</v>
       </c>
-      <c r="F13" t="s">
-        <v>3</v>
-      </c>
       <c r="G13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>228</v>
       </c>
@@ -1755,22 +2135,25 @@
         <v>Calle 62 # 130 54</v>
       </c>
       <c r="C14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D14" t="s">
         <v>111</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>290</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>6044278821</v>
       </c>
-      <c r="F14" t="s">
-        <v>3</v>
-      </c>
       <c r="G14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -1779,22 +2162,25 @@
         <v>Carrera 54 # 57 39</v>
       </c>
       <c r="C15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D15" t="s">
         <v>10</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>244</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>5127789</v>
       </c>
-      <c r="F15" t="s">
-        <v>3</v>
-      </c>
       <c r="G15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>138</v>
       </c>
@@ -1804,22 +2190,25 @@
 BARRIOSAN DIEGO</v>
       </c>
       <c r="C16" t="s">
+        <v>319</v>
+      </c>
+      <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>250</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>22327284</v>
       </c>
-      <c r="F16" t="s">
-        <v>3</v>
-      </c>
       <c r="G16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>207</v>
       </c>
@@ -1828,22 +2217,25 @@
         <v>Carrera 53 # 49 76</v>
       </c>
       <c r="C17" t="s">
+        <v>320</v>
+      </c>
+      <c r="D17" t="s">
         <v>90</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>293</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>6042311055</v>
       </c>
-      <c r="F17" t="s">
-        <v>3</v>
-      </c>
       <c r="G17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>196</v>
       </c>
@@ -1853,22 +2245,25 @@
 499</v>
       </c>
       <c r="C18" t="s">
+        <v>321</v>
+      </c>
+      <c r="D18" t="s">
         <v>79</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>283</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>3016195849</v>
       </c>
-      <c r="F18" t="s">
-        <v>3</v>
-      </c>
       <c r="G18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>141</v>
       </c>
@@ -1877,22 +2272,25 @@
         <v>Carrera 54 # 45 12</v>
       </c>
       <c r="C19" t="s">
+        <v>322</v>
+      </c>
+      <c r="D19" t="s">
         <v>24</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>253</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>5718449</v>
       </c>
-      <c r="F19" t="s">
-        <v>3</v>
-      </c>
       <c r="G19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -1901,22 +2299,25 @@
         <v>Calle 111 g # 64 a 89</v>
       </c>
       <c r="C20" t="s">
+        <v>323</v>
+      </c>
+      <c r="D20" t="s">
         <v>4</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>239</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>3192446804</v>
       </c>
-      <c r="F20" t="s">
-        <v>3</v>
-      </c>
       <c r="G20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>145</v>
       </c>
@@ -1926,22 +2327,25 @@
 Storage</v>
       </c>
       <c r="C21" t="s">
+        <v>324</v>
+      </c>
+      <c r="D21" t="s">
         <v>28</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>257</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>300</v>
       </c>
-      <c r="F21" t="s">
-        <v>3</v>
-      </c>
       <c r="G21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>180</v>
       </c>
@@ -1950,22 +2354,25 @@
         <v>Carrera 50 C # 10 sur 151</v>
       </c>
       <c r="C22" t="s">
+        <v>325</v>
+      </c>
+      <c r="D22" t="s">
         <v>63</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>242</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>3610010</v>
       </c>
-      <c r="F22" t="s">
-        <v>3</v>
-      </c>
       <c r="G22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>202</v>
       </c>
@@ -1974,22 +2381,25 @@
         <v>Carrera 79 # 38 A 44</v>
       </c>
       <c r="C23" t="s">
+        <v>326</v>
+      </c>
+      <c r="D23" t="s">
         <v>85</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>289</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>6045835290</v>
       </c>
-      <c r="F23" t="s">
-        <v>3</v>
-      </c>
       <c r="G23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>164</v>
       </c>
@@ -1998,22 +2408,25 @@
         <v>Calle 38 # 35 80</v>
       </c>
       <c r="C24" t="s">
+        <v>327</v>
+      </c>
+      <c r="D24" t="s">
         <v>47</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>263</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>3202850003</v>
       </c>
-      <c r="F24" t="s">
-        <v>3</v>
-      </c>
       <c r="G24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>178</v>
       </c>
@@ -2023,22 +2436,25 @@
 Edificio Bianco</v>
       </c>
       <c r="C25" t="s">
+        <v>328</v>
+      </c>
+      <c r="D25" t="s">
         <v>61</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>267</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>6044447570</v>
       </c>
-      <c r="F25" t="s">
-        <v>3</v>
-      </c>
       <c r="G25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>238</v>
       </c>
@@ -2047,22 +2463,25 @@
         <v>Calle 54 # 57 59</v>
       </c>
       <c r="C26" t="s">
+        <v>329</v>
+      </c>
+      <c r="D26" t="s">
         <v>20</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>298</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>3012687659</v>
       </c>
-      <c r="F26" t="s">
-        <v>3</v>
-      </c>
       <c r="G26" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>237</v>
       </c>
@@ -2071,22 +2490,25 @@
         <v>Calle 54 # 57 55</v>
       </c>
       <c r="C27" t="s">
+        <v>330</v>
+      </c>
+      <c r="D27" t="s">
         <v>120</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>297</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>3012687659</v>
       </c>
-      <c r="F27" t="s">
-        <v>3</v>
-      </c>
       <c r="G27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>204</v>
       </c>
@@ -2095,22 +2517,25 @@
         <v>Carrera 50 B # 39 104</v>
       </c>
       <c r="C28" t="s">
+        <v>331</v>
+      </c>
+      <c r="D28" t="s">
         <v>87</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>291</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>3136275706</v>
       </c>
-      <c r="F28" t="s">
-        <v>3</v>
-      </c>
       <c r="G28" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>209</v>
       </c>
@@ -2119,22 +2544,25 @@
         <v>Carrera 40 # 50 B 11</v>
       </c>
       <c r="C29" t="s">
+        <v>332</v>
+      </c>
+      <c r="D29" t="s">
         <v>92</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>291</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>3136275706</v>
       </c>
-      <c r="F29" t="s">
-        <v>3</v>
-      </c>
       <c r="G29" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>210</v>
       </c>
@@ -2143,22 +2571,25 @@
         <v>Calle 50 B # 38 80</v>
       </c>
       <c r="C30" t="s">
+        <v>333</v>
+      </c>
+      <c r="D30" t="s">
         <v>93</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>291</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>3136275706</v>
       </c>
-      <c r="F30" t="s">
-        <v>3</v>
-      </c>
       <c r="G30" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>152</v>
       </c>
@@ -2167,22 +2598,25 @@
         <v>Calle 94 # 51 B 33</v>
       </c>
       <c r="C31" t="s">
+        <v>334</v>
+      </c>
+      <c r="D31" t="s">
         <v>35</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>259</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>3234501778</v>
       </c>
-      <c r="F31" t="s">
-        <v>3</v>
-      </c>
       <c r="G31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>162</v>
       </c>
@@ -2191,22 +2625,25 @@
         <v>Carrera 82 # 49 f 68 apto401</v>
       </c>
       <c r="C32" t="s">
+        <v>335</v>
+      </c>
+      <c r="D32" t="s">
         <v>45</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>261</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>3216409583</v>
       </c>
-      <c r="F32" t="s">
-        <v>3</v>
-      </c>
       <c r="G32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>199</v>
       </c>
@@ -2215,22 +2652,25 @@
         <v>Calle 33 # 43 A 5</v>
       </c>
       <c r="C33" t="s">
+        <v>336</v>
+      </c>
+      <c r="D33" t="s">
         <v>82</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>286</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>3229827</v>
       </c>
-      <c r="F33" t="s">
-        <v>3</v>
-      </c>
       <c r="G33" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>197</v>
       </c>
@@ -2240,22 +2680,25 @@
 FLORIDANUEVA</v>
       </c>
       <c r="C34" t="s">
+        <v>337</v>
+      </c>
+      <c r="D34" t="s">
         <v>80</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>284</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>3137474778</v>
       </c>
-      <c r="F34" t="s">
-        <v>3</v>
-      </c>
       <c r="G34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>205</v>
       </c>
@@ -2264,22 +2707,25 @@
         <v>Calle 51 # 39 95</v>
       </c>
       <c r="C35" t="s">
+        <v>338</v>
+      </c>
+      <c r="D35" t="s">
         <v>88</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>291</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>3136275706</v>
       </c>
-      <c r="F35" t="s">
-        <v>3</v>
-      </c>
       <c r="G35" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -2289,22 +2735,25 @@
 Florida Parque Comercial</v>
       </c>
       <c r="C36" t="s">
+        <v>339</v>
+      </c>
+      <c r="D36" t="s">
         <v>31</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>258</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>3876000</v>
       </c>
-      <c r="F36" t="s">
-        <v>3</v>
-      </c>
       <c r="G36" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>153</v>
       </c>
@@ -2314,22 +2763,25 @@
 Edificio Centro de Negocios</v>
       </c>
       <c r="C37" t="s">
+        <v>340</v>
+      </c>
+      <c r="D37" t="s">
         <v>36</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>258</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>3876000</v>
       </c>
-      <c r="F37" t="s">
-        <v>3</v>
-      </c>
       <c r="G37" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>155</v>
       </c>
@@ -2339,22 +2791,25 @@
 Centro Comercial Arkadia</v>
       </c>
       <c r="C38" t="s">
+        <v>341</v>
+      </c>
+      <c r="D38" t="s">
         <v>38</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>258</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>3876000</v>
       </c>
-      <c r="F38" t="s">
-        <v>3</v>
-      </c>
       <c r="G38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>149</v>
       </c>
@@ -2363,22 +2818,25 @@
         <v>Carrera 65 # 50 12</v>
       </c>
       <c r="C39" t="s">
+        <v>342</v>
+      </c>
+      <c r="D39" t="s">
         <v>32</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>258</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>3876000</v>
       </c>
-      <c r="F39" t="s">
-        <v>3</v>
-      </c>
       <c r="G39" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>168</v>
       </c>
@@ -2388,22 +2846,25 @@
 CentroEmpresarila Ciudad del</v>
       </c>
       <c r="C40" t="s">
+        <v>343</v>
+      </c>
+      <c r="D40" t="s">
         <v>51</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>258</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>3876000</v>
       </c>
-      <c r="F40" t="s">
-        <v>3</v>
-      </c>
       <c r="G40" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>169</v>
       </c>
@@ -2413,22 +2874,25 @@
 9901, Centro Comercial del Este</v>
       </c>
       <c r="C41" t="s">
+        <v>344</v>
+      </c>
+      <c r="D41" t="s">
         <v>52</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>258</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>3876000</v>
       </c>
-      <c r="F41" t="s">
-        <v>3</v>
-      </c>
       <c r="G41" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>170</v>
       </c>
@@ -2438,22 +2902,25 @@
 224, Torre Comercial Demoda</v>
       </c>
       <c r="C42" t="s">
+        <v>345</v>
+      </c>
+      <c r="D42" t="s">
         <v>53</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>258</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>3876000</v>
       </c>
-      <c r="F42" t="s">
-        <v>3</v>
-      </c>
       <c r="G42" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>156</v>
       </c>
@@ -2463,22 +2930,25 @@
 Centro Comercial El Diamante</v>
       </c>
       <c r="C43" t="s">
+        <v>346</v>
+      </c>
+      <c r="D43" t="s">
         <v>39</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>258</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>3876000</v>
       </c>
-      <c r="F43" t="s">
-        <v>3</v>
-      </c>
       <c r="G43" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>173</v>
       </c>
@@ -2487,22 +2957,25 @@
         <v>Carrera 25 A # 1 A 45 sur</v>
       </c>
       <c r="C44" t="s">
+        <v>347</v>
+      </c>
+      <c r="D44" t="s">
         <v>56</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>258</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>3876000</v>
       </c>
-      <c r="F44" t="s">
-        <v>3</v>
-      </c>
       <c r="G44" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>161</v>
       </c>
@@ -2512,22 +2985,25 @@
 CentroComercial El Tesoro</v>
       </c>
       <c r="C45" t="s">
+        <v>348</v>
+      </c>
+      <c r="D45" t="s">
         <v>44</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>258</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>3876000</v>
       </c>
-      <c r="F45" t="s">
-        <v>3</v>
-      </c>
       <c r="G45" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>167</v>
       </c>
@@ -2537,22 +3013,25 @@
 Outlet Guayabal</v>
       </c>
       <c r="C46" t="s">
+        <v>349</v>
+      </c>
+      <c r="D46" t="s">
         <v>50</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>258</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>3876000</v>
       </c>
-      <c r="F46" t="s">
-        <v>3</v>
-      </c>
       <c r="G46" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>233</v>
       </c>
@@ -2561,22 +3040,25 @@
         <v>Calle 50 # 47 41</v>
       </c>
       <c r="C47" t="s">
+        <v>350</v>
+      </c>
+      <c r="D47" t="s">
         <v>116</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>258</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>3876000</v>
       </c>
-      <c r="F47" t="s">
-        <v>3</v>
-      </c>
       <c r="G47" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>147</v>
       </c>
@@ -2586,22 +3068,25 @@
 Centro Comercial La Central</v>
       </c>
       <c r="C48" t="s">
+        <v>351</v>
+      </c>
+      <c r="D48" t="s">
         <v>30</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>258</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>3876000</v>
       </c>
-      <c r="F48" t="s">
-        <v>3</v>
-      </c>
       <c r="G48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -2610,22 +3095,25 @@
         <v>Calle 30 A # 82 A 26 local4139</v>
       </c>
       <c r="C49" t="s">
+        <v>352</v>
+      </c>
+      <c r="D49" t="s">
         <v>29</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>258</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>3876000</v>
       </c>
-      <c r="F49" t="s">
-        <v>3</v>
-      </c>
       <c r="G49" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>229</v>
       </c>
@@ -2635,22 +3123,25 @@
 MallSantana, Local 201 A</v>
       </c>
       <c r="C50" t="s">
+        <v>353</v>
+      </c>
+      <c r="D50" t="s">
         <v>112</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>258</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>3876000</v>
       </c>
-      <c r="F50" t="s">
-        <v>3</v>
-      </c>
       <c r="G50" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>172</v>
       </c>
@@ -2659,22 +3150,25 @@
         <v>Carrera 45 # 69 55</v>
       </c>
       <c r="C51" t="s">
+        <v>354</v>
+      </c>
+      <c r="D51" t="s">
         <v>55</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>258</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>3876000</v>
       </c>
-      <c r="F51" t="s">
-        <v>3</v>
-      </c>
       <c r="G51" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>171</v>
       </c>
@@ -2683,22 +3177,25 @@
         <v>Calle 52 A # 50 46</v>
       </c>
       <c r="C52" t="s">
+        <v>355</v>
+      </c>
+      <c r="D52" t="s">
         <v>54</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>258</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>3876000</v>
       </c>
-      <c r="F52" t="s">
-        <v>3</v>
-      </c>
       <c r="G52" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>151</v>
       </c>
@@ -2708,22 +3205,25 @@
 Local5246, Centro Comercial</v>
       </c>
       <c r="C53" t="s">
+        <v>356</v>
+      </c>
+      <c r="D53" t="s">
         <v>34</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>258</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>3876000</v>
       </c>
-      <c r="F53" t="s">
-        <v>3</v>
-      </c>
       <c r="G53" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>150</v>
       </c>
@@ -2732,22 +3232,25 @@
         <v>Calle 38 # 48 51</v>
       </c>
       <c r="C54" t="s">
+        <v>357</v>
+      </c>
+      <c r="D54" t="s">
         <v>33</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>258</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>3876000</v>
       </c>
-      <c r="F54" t="s">
-        <v>3</v>
-      </c>
       <c r="G54" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>230</v>
       </c>
@@ -2757,22 +3260,25 @@
 CENTROCOMERCIAL</v>
       </c>
       <c r="C55" t="s">
+        <v>358</v>
+      </c>
+      <c r="D55" t="s">
         <v>113</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>258</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>3876000</v>
       </c>
-      <c r="F55" t="s">
-        <v>3</v>
-      </c>
       <c r="G55" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>231</v>
       </c>
@@ -2781,22 +3287,25 @@
         <v>Carrera 80 # 64 61 LocalL0091</v>
       </c>
       <c r="C56" t="s">
+        <v>359</v>
+      </c>
+      <c r="D56" t="s">
         <v>114</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>258</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>3876000</v>
       </c>
-      <c r="F56" t="s">
-        <v>3</v>
-      </c>
       <c r="G56" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>154</v>
       </c>
@@ -2805,22 +3314,25 @@
         <v>Carrera 80 # 79 C 157</v>
       </c>
       <c r="C57" t="s">
+        <v>360</v>
+      </c>
+      <c r="D57" t="s">
         <v>37</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>258</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>3876000</v>
       </c>
-      <c r="F57" t="s">
-        <v>3</v>
-      </c>
       <c r="G57" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>232</v>
       </c>
@@ -2829,22 +3341,25 @@
         <v>Carrera 78 SUR # 42 A 40 /42</v>
       </c>
       <c r="C58" t="s">
+        <v>361</v>
+      </c>
+      <c r="D58" t="s">
         <v>115</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>258</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>3876000</v>
       </c>
-      <c r="F58" t="s">
-        <v>3</v>
-      </c>
       <c r="G58" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>174</v>
       </c>
@@ -2854,22 +3369,25 @@
 CCSantafé</v>
       </c>
       <c r="C59" t="s">
+        <v>362</v>
+      </c>
+      <c r="D59" t="s">
         <v>57</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>258</v>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>3876000</v>
       </c>
-      <c r="F59" t="s">
-        <v>3</v>
-      </c>
       <c r="G59" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>157</v>
       </c>
@@ -2879,22 +3397,25 @@
 Local216, Centro Comercial</v>
       </c>
       <c r="C60" t="s">
+        <v>363</v>
+      </c>
+      <c r="D60" t="s">
         <v>40</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>258</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>3876000</v>
       </c>
-      <c r="F60" t="s">
-        <v>3</v>
-      </c>
       <c r="G60" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>176</v>
       </c>
@@ -2903,22 +3424,25 @@
         <v>Carrera 50 # 2 sur 189</v>
       </c>
       <c r="C61" t="s">
+        <v>364</v>
+      </c>
+      <c r="D61" t="s">
         <v>59</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>266</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>6579797</v>
       </c>
-      <c r="F61" t="s">
-        <v>3</v>
-      </c>
       <c r="G61" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>177</v>
       </c>
@@ -2927,22 +3451,25 @@
         <v>Calle 60 # 56 77</v>
       </c>
       <c r="C62" t="s">
+        <v>365</v>
+      </c>
+      <c r="D62" t="s">
         <v>60</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>266</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>6579797</v>
       </c>
-      <c r="F62" t="s">
-        <v>3</v>
-      </c>
       <c r="G62" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>183</v>
       </c>
@@ -2951,22 +3478,25 @@
         <v>Calle 49 # 45 39</v>
       </c>
       <c r="C63" t="s">
+        <v>366</v>
+      </c>
+      <c r="D63" t="s">
         <v>66</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>271</v>
       </c>
-      <c r="E63">
+      <c r="F63">
         <v>3137386728</v>
       </c>
-      <c r="F63" t="s">
-        <v>3</v>
-      </c>
       <c r="G63" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>193</v>
       </c>
@@ -2975,22 +3505,25 @@
         <v>Calle 51 # 64 B 21</v>
       </c>
       <c r="C64" t="s">
+        <v>367</v>
+      </c>
+      <c r="D64" t="s">
         <v>76</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>280</v>
       </c>
-      <c r="E64">
+      <c r="F64">
         <v>3175745860</v>
       </c>
-      <c r="F64" t="s">
-        <v>3</v>
-      </c>
       <c r="G64" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H64" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>195</v>
       </c>
@@ -3000,22 +3533,25 @@
 interior 701</v>
       </c>
       <c r="C65" t="s">
+        <v>368</v>
+      </c>
+      <c r="D65" t="s">
         <v>78</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>282</v>
       </c>
-      <c r="E65">
+      <c r="F65">
         <v>3128638824</v>
       </c>
-      <c r="F65" t="s">
-        <v>3</v>
-      </c>
       <c r="G65" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H65" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>136</v>
       </c>
@@ -3025,22 +3561,25 @@
 LOCAL3A</v>
       </c>
       <c r="C66" t="s">
+        <v>369</v>
+      </c>
+      <c r="D66" t="s">
         <v>19</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>248</v>
       </c>
-      <c r="E66">
+      <c r="F66">
         <v>2673707</v>
       </c>
-      <c r="F66" t="s">
-        <v>3</v>
-      </c>
       <c r="G66" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>236</v>
       </c>
@@ -3049,22 +3588,25 @@
         <v>Calle 50 # 38 45</v>
       </c>
       <c r="C67" t="s">
+        <v>370</v>
+      </c>
+      <c r="D67" t="s">
         <v>119</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>296</v>
       </c>
-      <c r="E67">
+      <c r="F67">
         <v>6043225424</v>
       </c>
-      <c r="F67" t="s">
-        <v>3</v>
-      </c>
       <c r="G67" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>128</v>
       </c>
@@ -3073,22 +3615,25 @@
         <v>Carrera 57 # 51 140</v>
       </c>
       <c r="C68" t="s">
+        <v>371</v>
+      </c>
+      <c r="D68" t="s">
         <v>11</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>244</v>
       </c>
-      <c r="E68">
+      <c r="F68">
         <v>5127789</v>
       </c>
-      <c r="F68" t="s">
-        <v>3</v>
-      </c>
       <c r="G68" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>194</v>
       </c>
@@ -3097,22 +3642,25 @@
         <v>Carrera 30 # 10 C 228</v>
       </c>
       <c r="C69" t="s">
+        <v>372</v>
+      </c>
+      <c r="D69" t="s">
         <v>77</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>281</v>
       </c>
-      <c r="E69">
+      <c r="F69">
         <v>3127085363</v>
       </c>
-      <c r="F69" t="s">
-        <v>3</v>
-      </c>
       <c r="G69" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>208</v>
       </c>
@@ -3122,22 +3670,25 @@
 4</v>
       </c>
       <c r="C70" t="s">
+        <v>373</v>
+      </c>
+      <c r="D70" t="s">
         <v>91</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>294</v>
       </c>
-      <c r="E70">
+      <c r="F70">
         <v>6151515</v>
       </c>
-      <c r="F70" t="s">
-        <v>3</v>
-      </c>
       <c r="G70" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>159</v>
       </c>
@@ -3147,22 +3698,25 @@
 Industriales</v>
       </c>
       <c r="C71" t="s">
+        <v>374</v>
+      </c>
+      <c r="D71" t="s">
         <v>42</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>260</v>
       </c>
-      <c r="E71">
+      <c r="F71">
         <v>3904100</v>
       </c>
-      <c r="F71" t="s">
-        <v>3</v>
-      </c>
       <c r="G71" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>158</v>
       </c>
@@ -3172,22 +3726,25 @@
 Molinos local 1131</v>
       </c>
       <c r="C72" t="s">
+        <v>375</v>
+      </c>
+      <c r="D72" t="s">
         <v>41</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>260</v>
       </c>
-      <c r="E72">
+      <c r="F72">
         <v>3904100</v>
       </c>
-      <c r="F72" t="s">
-        <v>3</v>
-      </c>
       <c r="G72" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>160</v>
       </c>
@@ -3196,22 +3753,25 @@
         <v>Calle 44 # 65 100</v>
       </c>
       <c r="C73" t="s">
+        <v>376</v>
+      </c>
+      <c r="D73" t="s">
         <v>43</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>260</v>
       </c>
-      <c r="E73">
+      <c r="F73">
         <v>3904100</v>
       </c>
-      <c r="F73" t="s">
-        <v>3</v>
-      </c>
       <c r="G73" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H73" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>142</v>
       </c>
@@ -3221,22 +3781,25 @@
 AUTOPISTAMEDELLIN</v>
       </c>
       <c r="C74" t="s">
+        <v>377</v>
+      </c>
+      <c r="D74" t="s">
         <v>25</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>254</v>
       </c>
-      <c r="E74">
+      <c r="F74">
         <v>3208361305</v>
       </c>
-      <c r="F74" t="s">
-        <v>3</v>
-      </c>
       <c r="G74" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>133</v>
       </c>
@@ -3245,22 +3808,25 @@
         <v>Carrera 43 A # 11 B 145 101</v>
       </c>
       <c r="C75" t="s">
+        <v>378</v>
+      </c>
+      <c r="D75" t="s">
         <v>16</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>246</v>
       </c>
-      <c r="E75">
+      <c r="F75">
         <v>3167700</v>
       </c>
-      <c r="F75" t="s">
-        <v>3</v>
-      </c>
       <c r="G75" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>188</v>
       </c>
@@ -3269,22 +3835,25 @@
         <v>Carrera 30 # 30 46</v>
       </c>
       <c r="C76" t="s">
+        <v>379</v>
+      </c>
+      <c r="D76" t="s">
         <v>71</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>275</v>
       </c>
-      <c r="E76">
+      <c r="F76">
         <v>8498152</v>
       </c>
-      <c r="F76" t="s">
-        <v>3</v>
-      </c>
       <c r="G76" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>191</v>
       </c>
@@ -3293,22 +3862,25 @@
         <v>Calle 50 # 68 65 Local18</v>
       </c>
       <c r="C77" t="s">
+        <v>380</v>
+      </c>
+      <c r="D77" t="s">
         <v>74</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>278</v>
       </c>
-      <c r="E77">
+      <c r="F77">
         <v>3006171312</v>
       </c>
-      <c r="F77" t="s">
-        <v>3</v>
-      </c>
       <c r="G77" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H77" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>134</v>
       </c>
@@ -3317,22 +3889,25 @@
         <v>Carrera 43 A # 11 B 145</v>
       </c>
       <c r="C78" t="s">
+        <v>378</v>
+      </c>
+      <c r="D78" t="s">
         <v>17</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>246</v>
       </c>
-      <c r="E78">
+      <c r="F78">
         <v>3167700</v>
       </c>
-      <c r="F78" t="s">
-        <v>3</v>
-      </c>
       <c r="G78" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H78" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>143</v>
       </c>
@@ -3342,22 +3917,25 @@
 ROSITA INT. 301</v>
       </c>
       <c r="C79" t="s">
+        <v>381</v>
+      </c>
+      <c r="D79" t="s">
         <v>26</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>255</v>
       </c>
-      <c r="E79">
+      <c r="F79">
         <v>2317995</v>
       </c>
-      <c r="F79" t="s">
-        <v>3</v>
-      </c>
       <c r="G79" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H79" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>126</v>
       </c>
@@ -3366,22 +3944,25 @@
         <v>Carrera 74 # 53 21 LOCAL21</v>
       </c>
       <c r="C80" t="s">
+        <v>382</v>
+      </c>
+      <c r="D80" t="s">
         <v>9</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>243</v>
       </c>
-      <c r="E80">
+      <c r="F80">
         <v>4445268</v>
       </c>
-      <c r="F80" t="s">
-        <v>3</v>
-      </c>
       <c r="G80" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H80" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>125</v>
       </c>
@@ -3390,22 +3971,25 @@
         <v>Calle 37 # 80 36 LOCAL128</v>
       </c>
       <c r="C81" t="s">
+        <v>383</v>
+      </c>
+      <c r="D81" t="s">
         <v>8</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>243</v>
       </c>
-      <c r="E81">
+      <c r="F81">
         <v>4445268</v>
       </c>
-      <c r="F81" t="s">
-        <v>3</v>
-      </c>
       <c r="G81" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H81" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>182</v>
       </c>
@@ -3414,22 +3998,25 @@
         <v>Calle 20 sur # 27 124</v>
       </c>
       <c r="C82" t="s">
+        <v>384</v>
+      </c>
+      <c r="D82" t="s">
         <v>65</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>270</v>
       </c>
-      <c r="E82">
+      <c r="F82">
         <v>4449303</v>
       </c>
-      <c r="F82" t="s">
-        <v>3</v>
-      </c>
       <c r="G82" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>137</v>
       </c>
@@ -3438,22 +4025,25 @@
         <v>Calle 54 # 57 59</v>
       </c>
       <c r="C83" t="s">
+        <v>329</v>
+      </c>
+      <c r="D83" t="s">
         <v>20</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>249</v>
       </c>
-      <c r="E83">
+      <c r="F83">
         <v>4798852</v>
       </c>
-      <c r="F83" t="s">
-        <v>3</v>
-      </c>
       <c r="G83" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H83" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>190</v>
       </c>
@@ -3462,22 +4052,25 @@
         <v>Calle 6 SUR # 79 150</v>
       </c>
       <c r="C84" t="s">
+        <v>385</v>
+      </c>
+      <c r="D84" t="s">
         <v>73</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>277</v>
       </c>
-      <c r="E84">
+      <c r="F84">
         <v>3008333787</v>
       </c>
-      <c r="F84" t="s">
-        <v>3</v>
-      </c>
       <c r="G84" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>185</v>
       </c>
@@ -3486,22 +4079,25 @@
         <v>vereda santa elena</v>
       </c>
       <c r="C85" t="s">
+        <v>386</v>
+      </c>
+      <c r="D85" t="s">
         <v>68</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>273</v>
       </c>
-      <c r="E85">
+      <c r="F85">
         <v>3127367291</v>
       </c>
-      <c r="F85" t="s">
-        <v>3</v>
-      </c>
       <c r="G85" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>140</v>
       </c>
@@ -3510,22 +4106,25 @@
         <v>Calle 48 # 54 15</v>
       </c>
       <c r="C86" t="s">
+        <v>387</v>
+      </c>
+      <c r="D86" t="s">
         <v>23</v>
       </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
         <v>252</v>
       </c>
-      <c r="E86">
+      <c r="F86">
         <v>5112042</v>
       </c>
-      <c r="F86" t="s">
-        <v>3</v>
-      </c>
       <c r="G86" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>139</v>
       </c>
@@ -3534,22 +4133,25 @@
         <v>Carrera 64 B # 35 71 of1103</v>
       </c>
       <c r="C87" t="s">
+        <v>388</v>
+      </c>
+      <c r="D87" t="s">
         <v>22</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>251</v>
       </c>
-      <c r="E87">
+      <c r="F87">
         <v>5085275</v>
       </c>
-      <c r="F87" t="s">
-        <v>3</v>
-      </c>
       <c r="G87" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H87" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>144</v>
       </c>
@@ -3559,22 +4161,25 @@
 SANANTONIO DE PRADO</v>
       </c>
       <c r="C88" t="s">
+        <v>389</v>
+      </c>
+      <c r="D88" t="s">
         <v>27</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>256</v>
       </c>
-      <c r="E88">
+      <c r="F88">
         <v>573370067</v>
       </c>
-      <c r="F88" t="s">
-        <v>3</v>
-      </c>
       <c r="G88" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H88" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>181</v>
       </c>
@@ -3583,22 +4188,25 @@
         <v>Calle 20 # 35 120</v>
       </c>
       <c r="C89" t="s">
+        <v>390</v>
+      </c>
+      <c r="D89" t="s">
         <v>64</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>269</v>
       </c>
-      <c r="E89">
+      <c r="F89">
         <v>4443075</v>
       </c>
-      <c r="F89" t="s">
-        <v>3</v>
-      </c>
       <c r="G89" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>192</v>
       </c>
@@ -3607,22 +4215,25 @@
         <v>Carrera 147 # 67 B 67</v>
       </c>
       <c r="C90" t="s">
+        <v>391</v>
+      </c>
+      <c r="D90" t="s">
         <v>75</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
         <v>279</v>
       </c>
-      <c r="E90">
+      <c r="F90">
         <v>2299183</v>
       </c>
-      <c r="F90" t="s">
-        <v>3</v>
-      </c>
       <c r="G90" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>175</v>
       </c>
@@ -3631,22 +4242,25 @@
         <v>Carrera 52 # 109 b 33</v>
       </c>
       <c r="C91" t="s">
+        <v>392</v>
+      </c>
+      <c r="D91" t="s">
         <v>58</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>265</v>
       </c>
-      <c r="E91">
+      <c r="F91">
         <v>4485871</v>
       </c>
-      <c r="F91" t="s">
-        <v>3</v>
-      </c>
       <c r="G91" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H91" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>124</v>
       </c>
@@ -3655,22 +4269,25 @@
         <v>Carrera 50 c # 10 sur 199</v>
       </c>
       <c r="C92" t="s">
+        <v>325</v>
+      </c>
+      <c r="D92" t="s">
         <v>7</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>242</v>
       </c>
-      <c r="E92">
+      <c r="F92">
         <v>3610010</v>
       </c>
-      <c r="F92" t="s">
-        <v>3</v>
-      </c>
       <c r="G92" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H92" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>163</v>
       </c>
@@ -3679,22 +4296,25 @@
         <v>Carrera 48 # 7 332</v>
       </c>
       <c r="C93" t="s">
+        <v>393</v>
+      </c>
+      <c r="D93" t="s">
         <v>46</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>262</v>
       </c>
-      <c r="E93">
+      <c r="F93">
         <v>3159265983</v>
       </c>
-      <c r="F93" t="s">
-        <v>3</v>
-      </c>
       <c r="G93" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H93" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>186</v>
       </c>
@@ -3703,22 +4323,25 @@
         <v>Transversal 40 # 74 A 40 Local2</v>
       </c>
       <c r="C94" t="s">
+        <v>394</v>
+      </c>
+      <c r="D94" t="s">
         <v>69</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>262</v>
       </c>
-      <c r="E94">
+      <c r="F94">
         <v>3159265983</v>
       </c>
-      <c r="F94" t="s">
-        <v>3</v>
-      </c>
       <c r="G94" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H94" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>206</v>
       </c>
@@ -3728,22 +4351,25 @@
 BARRIOLAURELES</v>
       </c>
       <c r="C95" t="s">
+        <v>395</v>
+      </c>
+      <c r="D95" t="s">
         <v>89</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>292</v>
       </c>
-      <c r="E95">
+      <c r="F95">
         <v>3116800178</v>
       </c>
-      <c r="F95" t="s">
-        <v>3</v>
-      </c>
       <c r="G95" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H95" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>165</v>
       </c>
@@ -3752,22 +4378,25 @@
         <v>Calle 2 # 52 37</v>
       </c>
       <c r="C96" t="s">
+        <v>396</v>
+      </c>
+      <c r="D96" t="s">
         <v>48</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>264</v>
       </c>
-      <c r="E96">
+      <c r="F96">
         <v>3176669406</v>
       </c>
-      <c r="F96" t="s">
-        <v>3</v>
-      </c>
       <c r="G96" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H96" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>166</v>
       </c>
@@ -3776,22 +4405,25 @@
         <v>Carrera 87 # 47 DD 72</v>
       </c>
       <c r="C97" t="s">
+        <v>397</v>
+      </c>
+      <c r="D97" t="s">
         <v>49</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>264</v>
       </c>
-      <c r="E97">
+      <c r="F97">
         <v>3176669406</v>
       </c>
-      <c r="F97" t="s">
-        <v>3</v>
-      </c>
       <c r="G97" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H97" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>129</v>
       </c>
@@ -3800,22 +4432,25 @@
         <v>Carrera 57 # 51 30</v>
       </c>
       <c r="C98" t="s">
+        <v>398</v>
+      </c>
+      <c r="D98" t="s">
         <v>12</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>244</v>
       </c>
-      <c r="E98">
+      <c r="F98">
         <v>5127789</v>
       </c>
-      <c r="F98" t="s">
-        <v>3</v>
-      </c>
       <c r="G98" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H98" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>222</v>
       </c>
@@ -3824,22 +4459,25 @@
         <v>Carrera 50 A # 93 26</v>
       </c>
       <c r="C99" t="s">
+        <v>399</v>
+      </c>
+      <c r="D99" t="s">
         <v>105</v>
       </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
         <v>295</v>
       </c>
-      <c r="E99">
+      <c r="F99">
         <v>3017574775</v>
       </c>
-      <c r="F99" t="s">
-        <v>3</v>
-      </c>
       <c r="G99" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H99" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>220</v>
       </c>
@@ -3848,22 +4486,25 @@
         <v>Calle 25 # 65 A 38</v>
       </c>
       <c r="C100" t="s">
+        <v>400</v>
+      </c>
+      <c r="D100" t="s">
         <v>103</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>295</v>
       </c>
-      <c r="E100">
+      <c r="F100">
         <v>3017574775</v>
       </c>
-      <c r="F100" t="s">
-        <v>3</v>
-      </c>
       <c r="G100" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H100" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>227</v>
       </c>
@@ -3872,22 +4513,25 @@
         <v>Carrera 88 # 39 53</v>
       </c>
       <c r="C101" t="s">
+        <v>401</v>
+      </c>
+      <c r="D101" t="s">
         <v>110</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>295</v>
       </c>
-      <c r="E101">
+      <c r="F101">
         <v>3017574775</v>
       </c>
-      <c r="F101" t="s">
-        <v>3</v>
-      </c>
       <c r="G101" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H101" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>218</v>
       </c>
@@ -3896,22 +4540,25 @@
         <v>Carrera 64 A # 103 29</v>
       </c>
       <c r="C102" t="s">
+        <v>402</v>
+      </c>
+      <c r="D102" t="s">
         <v>101</v>
       </c>
-      <c r="D102" t="s">
+      <c r="E102" t="s">
         <v>295</v>
       </c>
-      <c r="E102">
+      <c r="F102">
         <v>3017574775</v>
       </c>
-      <c r="F102" t="s">
-        <v>3</v>
-      </c>
       <c r="G102" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H102" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>234</v>
       </c>
@@ -3920,22 +4567,25 @@
         <v>Calle 29 A # 83 A 10</v>
       </c>
       <c r="C103" t="s">
+        <v>403</v>
+      </c>
+      <c r="D103" t="s">
         <v>117</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>295</v>
       </c>
-      <c r="E103">
+      <c r="F103">
         <v>3017574775</v>
       </c>
-      <c r="F103" t="s">
-        <v>3</v>
-      </c>
       <c r="G103" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H103" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>215</v>
       </c>
@@ -3944,22 +4594,25 @@
         <v>Calle 49 # 33 30</v>
       </c>
       <c r="C104" t="s">
+        <v>404</v>
+      </c>
+      <c r="D104" t="s">
         <v>98</v>
       </c>
-      <c r="D104" t="s">
+      <c r="E104" t="s">
         <v>295</v>
       </c>
-      <c r="E104">
+      <c r="F104">
         <v>3017574775</v>
       </c>
-      <c r="F104" t="s">
-        <v>3</v>
-      </c>
       <c r="G104" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H104" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>212</v>
       </c>
@@ -3968,22 +4621,25 @@
         <v>Calle 49 # 80 29</v>
       </c>
       <c r="C105" t="s">
+        <v>405</v>
+      </c>
+      <c r="D105" t="s">
         <v>95</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" t="s">
         <v>295</v>
       </c>
-      <c r="E105">
+      <c r="F105">
         <v>3017574775</v>
       </c>
-      <c r="F105" t="s">
-        <v>3</v>
-      </c>
       <c r="G105" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H105" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>235</v>
       </c>
@@ -3992,22 +4648,25 @@
         <v>Calle 8 # 45 38</v>
       </c>
       <c r="C106" t="s">
+        <v>406</v>
+      </c>
+      <c r="D106" t="s">
         <v>118</v>
       </c>
-      <c r="D106" t="s">
+      <c r="E106" t="s">
         <v>295</v>
       </c>
-      <c r="E106">
+      <c r="F106">
         <v>3017574775</v>
       </c>
-      <c r="F106" t="s">
-        <v>3</v>
-      </c>
       <c r="G106" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H106" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>214</v>
       </c>
@@ -4016,22 +4675,25 @@
         <v>Calle 96 # 67 52</v>
       </c>
       <c r="C107" t="s">
+        <v>407</v>
+      </c>
+      <c r="D107" t="s">
         <v>97</v>
       </c>
-      <c r="D107" t="s">
+      <c r="E107" t="s">
         <v>295</v>
       </c>
-      <c r="E107">
+      <c r="F107">
         <v>3017574775</v>
       </c>
-      <c r="F107" t="s">
-        <v>3</v>
-      </c>
       <c r="G107" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>211</v>
       </c>
@@ -4040,22 +4702,25 @@
         <v>Calle 44 A # 71 72</v>
       </c>
       <c r="C108" t="s">
+        <v>408</v>
+      </c>
+      <c r="D108" t="s">
         <v>94</v>
       </c>
-      <c r="D108" t="s">
+      <c r="E108" t="s">
         <v>295</v>
       </c>
-      <c r="E108">
+      <c r="F108">
         <v>3017574775</v>
       </c>
-      <c r="F108" t="s">
-        <v>3</v>
-      </c>
       <c r="G108" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H108" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>225</v>
       </c>
@@ -4064,22 +4729,25 @@
         <v>Carrera 52 # 14 SUR 75</v>
       </c>
       <c r="C109" t="s">
+        <v>409</v>
+      </c>
+      <c r="D109" t="s">
         <v>108</v>
       </c>
-      <c r="D109" t="s">
+      <c r="E109" t="s">
         <v>295</v>
       </c>
-      <c r="E109">
+      <c r="F109">
         <v>3017574775</v>
       </c>
-      <c r="F109" t="s">
-        <v>3</v>
-      </c>
       <c r="G109" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H109" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>221</v>
       </c>
@@ -4088,22 +4756,25 @@
         <v>Calle 32 F # 75 C 145</v>
       </c>
       <c r="C110" t="s">
+        <v>410</v>
+      </c>
+      <c r="D110" t="s">
         <v>104</v>
       </c>
-      <c r="D110" t="s">
+      <c r="E110" t="s">
         <v>295</v>
       </c>
-      <c r="E110">
+      <c r="F110">
         <v>3017574775</v>
       </c>
-      <c r="F110" t="s">
-        <v>3</v>
-      </c>
       <c r="G110" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H110" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>219</v>
       </c>
@@ -4112,22 +4783,25 @@
         <v>Calle 75 # 72 B 227</v>
       </c>
       <c r="C111" t="s">
+        <v>411</v>
+      </c>
+      <c r="D111" t="s">
         <v>102</v>
       </c>
-      <c r="D111" t="s">
+      <c r="E111" t="s">
         <v>295</v>
       </c>
-      <c r="E111">
+      <c r="F111">
         <v>3017574775</v>
       </c>
-      <c r="F111" t="s">
-        <v>3</v>
-      </c>
       <c r="G111" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H111" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>223</v>
       </c>
@@ -4136,22 +4810,25 @@
         <v>Carrera 86 # 64 45</v>
       </c>
       <c r="C112" t="s">
+        <v>412</v>
+      </c>
+      <c r="D112" t="s">
         <v>106</v>
       </c>
-      <c r="D112" t="s">
+      <c r="E112" t="s">
         <v>295</v>
       </c>
-      <c r="E112">
+      <c r="F112">
         <v>3017574775</v>
       </c>
-      <c r="F112" t="s">
-        <v>3</v>
-      </c>
       <c r="G112" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H112" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>224</v>
       </c>
@@ -4160,22 +4837,25 @@
         <v>Calle 77 BB # 82 107</v>
       </c>
       <c r="C113" t="s">
+        <v>413</v>
+      </c>
+      <c r="D113" t="s">
         <v>107</v>
       </c>
-      <c r="D113" t="s">
+      <c r="E113" t="s">
         <v>295</v>
       </c>
-      <c r="E113">
+      <c r="F113">
         <v>3017574775</v>
       </c>
-      <c r="F113" t="s">
-        <v>3</v>
-      </c>
       <c r="G113" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H113" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>216</v>
       </c>
@@ -4184,22 +4864,25 @@
         <v>Carrera 78 S # 19 13</v>
       </c>
       <c r="C114" t="s">
+        <v>361</v>
+      </c>
+      <c r="D114" t="s">
         <v>99</v>
       </c>
-      <c r="D114" t="s">
+      <c r="E114" t="s">
         <v>295</v>
       </c>
-      <c r="E114">
+      <c r="F114">
         <v>3017574775</v>
       </c>
-      <c r="F114" t="s">
-        <v>3</v>
-      </c>
       <c r="G114" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H114" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>217</v>
       </c>
@@ -4208,22 +4891,25 @@
         <v>Calle 40 # 105 102</v>
       </c>
       <c r="C115" t="s">
+        <v>414</v>
+      </c>
+      <c r="D115" t="s">
         <v>100</v>
       </c>
-      <c r="D115" t="s">
+      <c r="E115" t="s">
         <v>295</v>
       </c>
-      <c r="E115">
+      <c r="F115">
         <v>3017574775</v>
       </c>
-      <c r="F115" t="s">
-        <v>3</v>
-      </c>
       <c r="G115" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H115" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>226</v>
       </c>
@@ -4232,22 +4918,25 @@
         <v>Calle 100 # 46 A 28</v>
       </c>
       <c r="C116" t="s">
+        <v>415</v>
+      </c>
+      <c r="D116" t="s">
         <v>109</v>
       </c>
-      <c r="D116" t="s">
+      <c r="E116" t="s">
         <v>295</v>
       </c>
-      <c r="E116">
+      <c r="F116">
         <v>3017574775</v>
       </c>
-      <c r="F116" t="s">
-        <v>3</v>
-      </c>
       <c r="G116" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H116" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>213</v>
       </c>
@@ -4256,22 +4945,25 @@
         <v>Carrera 87 # 47 DD 61</v>
       </c>
       <c r="C117" t="s">
+        <v>397</v>
+      </c>
+      <c r="D117" t="s">
         <v>96</v>
       </c>
-      <c r="D117" t="s">
+      <c r="E117" t="s">
         <v>295</v>
       </c>
-      <c r="E117">
+      <c r="F117">
         <v>3017574775</v>
       </c>
-      <c r="F117" t="s">
-        <v>3</v>
-      </c>
       <c r="G117" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H117" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>123</v>
       </c>
@@ -4280,22 +4972,25 @@
         <v>Calle 32 # 48 45</v>
       </c>
       <c r="C118" t="s">
+        <v>416</v>
+      </c>
+      <c r="D118" t="s">
         <v>6</v>
       </c>
-      <c r="D118" t="s">
+      <c r="E118" t="s">
         <v>241</v>
       </c>
-      <c r="E118" t="s">
+      <c r="F118" t="s">
         <v>299</v>
       </c>
-      <c r="F118" t="s">
-        <v>3</v>
-      </c>
       <c r="G118" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H118" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>184</v>
       </c>
@@ -4305,25 +5000,29 @@
 POBLADO</v>
       </c>
       <c r="C119" t="s">
+        <v>417</v>
+      </c>
+      <c r="D119" t="s">
         <v>67</v>
       </c>
-      <c r="D119" t="s">
+      <c r="E119" t="s">
         <v>272</v>
       </c>
-      <c r="E119">
+      <c r="F119">
         <v>4440855</v>
       </c>
-      <c r="F119" t="s">
-        <v>3</v>
-      </c>
       <c r="G119" t="s">
+        <v>3</v>
+      </c>
+      <c r="H119" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>